<commit_message>
code check In 30 sept
</commit_message>
<xml_diff>
--- a/MyMojioWebsite/bin/com/mojio/xls/SignIn.xlsx
+++ b/MyMojioWebsite/bin/com/mojio/xls/SignIn.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="771" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="771" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="107">
   <si>
     <t>TCID</t>
   </si>
@@ -144,76 +144,79 @@
     <t>Write the password</t>
   </si>
   <si>
+    <t>signInPasswordId</t>
+  </si>
+  <si>
+    <t>col|Sign_In_Password</t>
+  </si>
+  <si>
+    <t>TS006</t>
+  </si>
+  <si>
+    <t>Click on Submit button</t>
+  </si>
+  <si>
+    <t>clickByXpath</t>
+  </si>
+  <si>
+    <t>SubmitXpath</t>
+  </si>
+  <si>
+    <t>TS007</t>
+  </si>
+  <si>
+    <t>Verify the dashboard page</t>
+  </si>
+  <si>
+    <t>col|Dashboard_Page</t>
+  </si>
+  <si>
+    <t>TS008</t>
+  </si>
+  <si>
+    <t>Click on settings icon</t>
+  </si>
+  <si>
+    <t>clickByID</t>
+  </si>
+  <si>
+    <t>settingsId</t>
+  </si>
+  <si>
+    <t>TS009</t>
+  </si>
+  <si>
+    <t>Click on log out</t>
+  </si>
+  <si>
+    <t>logOutXpath</t>
+  </si>
+  <si>
+    <t>TS010</t>
+  </si>
+  <si>
+    <t>Verify the sign in user name blank error</t>
+  </si>
+  <si>
+    <t>verifyTextByXpath</t>
+  </si>
+  <si>
+    <t>signInUsernameErrorXpath</t>
+  </si>
+  <si>
+    <t>col|Field_Blank</t>
+  </si>
+  <si>
+    <t>Verify the password blank error</t>
+  </si>
+  <si>
+    <t>SignInPasswordErrorXpath</t>
+  </si>
+  <si>
     <t>writeInInputByXpath</t>
   </si>
   <si>
     <t>signInPasswordXpath</t>
-  </si>
-  <si>
-    <t>col|Sign_In_Password</t>
-  </si>
-  <si>
-    <t>TS006</t>
-  </si>
-  <si>
-    <t>Click on Submit button</t>
-  </si>
-  <si>
-    <t>clickByXpath</t>
-  </si>
-  <si>
-    <t>SubmitXpath</t>
-  </si>
-  <si>
-    <t>TS007</t>
-  </si>
-  <si>
-    <t>Verify the dashboard page</t>
-  </si>
-  <si>
-    <t>col|Dashboard_Page</t>
-  </si>
-  <si>
-    <t>TS008</t>
-  </si>
-  <si>
-    <t>Click on settings icon</t>
-  </si>
-  <si>
-    <t>clickByID</t>
-  </si>
-  <si>
-    <t>settingsId</t>
-  </si>
-  <si>
-    <t>TS009</t>
-  </si>
-  <si>
-    <t>Click on log out</t>
-  </si>
-  <si>
-    <t>logOutXpath</t>
-  </si>
-  <si>
-    <t>TS010</t>
-  </si>
-  <si>
-    <t>Verify the sign in user name blank error</t>
-  </si>
-  <si>
-    <t>verifyTextByXpath</t>
-  </si>
-  <si>
-    <t>signInUsernameErrorXpath</t>
-  </si>
-  <si>
-    <t>col|Field_Blank</t>
-  </si>
-  <si>
-    <t>Verify the password blank error</t>
-  </si>
-  <si>
-    <t>SignInPasswordErrorXpath</t>
   </si>
   <si>
     <t>Verify the User name blank error</t>
@@ -349,9 +352,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="GENERAL"/>
+  <numFmts count="1">
+    <numFmt formatCode="GENERAL" numFmtId="164"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -468,7 +470,7 @@
       <protection hidden="false" locked="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -489,11 +491,15 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="0" numFmtId="165" xfId="0">
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="4" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -601,16 +607,16 @@
   </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="G10" activeCellId="0" pane="topLeft" sqref="G10"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="G10" activeCellId="1" pane="topLeft" sqref="C2:F8 G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="28.1428571428571" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="0" width="25.4234693877551" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="0" width="25.2908163265306" collapsed="true"/>
-    <col min="4" max="1025" hidden="false" style="0" width="8.6734693877551" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.1428571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.4234693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.2908163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.6734693877551"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="1">
@@ -724,34 +730,34 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="C2:F8 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="45.4285714285714" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="0" width="34.5408163265306" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="0" width="22.8520408163265" collapsed="true"/>
-    <col min="4" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.4285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.5408163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.8520408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="2">
-      <c r="A2" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>103</v>
+      <c r="A2" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>104</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>4</v>
@@ -776,48 +782,48 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D7" activeCellId="0" pane="topLeft" sqref="D7"/>
+      <selection activeCell="D7" activeCellId="0" pane="topLeft" sqref="C2:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="45.0255102040816" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="0" width="34.4030612244898" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="0" width="34.2704081632653" collapsed="true"/>
-    <col min="4" max="4" hidden="false" style="0" width="45.8316326530612" collapsed="true"/>
-    <col min="5" max="5" hidden="false" style="0" width="22.8520408163265" collapsed="true"/>
-    <col min="6" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.0255102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.4030612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.2704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.8316326530612"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.8520408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>2</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="2">
-      <c r="A2" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>103</v>
+      <c r="A2" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>104</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>105</v>
+        <v>91</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>106</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>4</v>
@@ -825,7 +831,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="mojio.2@optimusinfo.com" ref="C2" r:id="rId58"/>
+    <hyperlink display="mojio.2@optimusinfo.com" ref="C2" r:id="rId1"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -844,22 +850,22 @@
   </sheetPr>
   <dimension ref="1:58"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A16" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A53" activeCellId="0" pane="topLeft" sqref="A53"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="F8" activeCellId="0" pane="topLeft" sqref="C2:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="4" width="28.2857142857143" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="4" width="8.56632653061224" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="4" width="41.6683673469388" collapsed="true"/>
-    <col min="4" max="4" hidden="false" style="4" width="29.030612244898" collapsed="true"/>
-    <col min="5" max="5" hidden="false" style="4" width="34.0102040816326" collapsed="true"/>
-    <col min="6" max="6" hidden="false" style="4" width="29.3010204081633" collapsed="true"/>
-    <col min="7" max="7" hidden="false" style="4" width="16.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" hidden="false" style="4" width="7.51171875" collapsed="true"/>
-    <col min="9" max="1011" hidden="false" style="4" width="8.6734693877551" collapsed="true"/>
-    <col min="1012" max="1025" hidden="false" style="0" width="8.6734693877551" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="28.2857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="8.56632653061224"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="4" width="41.6683673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="4" width="29.030612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="4" width="34.0102040816326"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="29.3010204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="16"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="4" width="7.51530612244898"/>
+    <col collapsed="false" hidden="false" max="1011" min="9" style="4" width="8.6734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1012" style="0" width="8.6734693877551"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="1">
@@ -989,13 +995,13 @@
         <v>38</v>
       </c>
       <c r="D6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>40</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>41</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="4" t="s">
@@ -1007,16 +1013,16 @@
         <v>3</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -1029,17 +1035,17 @@
         <v>3</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>47</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>30</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="4" t="s">
@@ -1051,16 +1057,16 @@
         <v>3</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="D9" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="E9" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>52</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
@@ -1073,16 +1079,16 @@
         <v>3</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="D10" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>55</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
@@ -1095,7 +1101,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>29</v>
@@ -1113,160 +1119,160 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="12">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7" t="s">
+      <c r="E12" s="8"/>
+      <c r="F12" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="7"/>
-      <c r="H12" t="s">
+      <c r="G12" s="8"/>
+      <c r="H12" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="13">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7" t="s">
+      <c r="E13" s="8"/>
+      <c r="F13" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G13" s="7"/>
-      <c r="H13" t="s">
+      <c r="G13" s="8"/>
+      <c r="H13" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="14">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="E14" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" t="s">
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="15">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="E15" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="F15" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="G15" s="8"/>
+      <c r="H15" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="16">
+      <c r="A16" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="G15" s="7"/>
-      <c r="H15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="16">
-      <c r="A16" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="7" t="s">
+      <c r="D16" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="G16" s="7"/>
-      <c r="H16" t="s">
+      <c r="F16" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G16" s="8"/>
+      <c r="H16" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="17">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8" t="s">
+      <c r="E17" s="9"/>
+      <c r="F17" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="G17" s="8"/>
-      <c r="H17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="18" s="9">
-      <c r="A18" s="8" t="s">
+      <c r="G17" s="9"/>
+      <c r="H17" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="18" s="10">
+      <c r="A18" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8" t="s">
+      <c r="E18" s="9"/>
+      <c r="F18" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G18" s="8"/>
-      <c r="H18" t="s">
+      <c r="G18" s="9"/>
+      <c r="H18" s="10" t="s">
         <v>23</v>
       </c>
       <c r="ALX18" s="0"/>
@@ -1283,27 +1289,27 @@
       <c r="AMI18" s="0"/>
       <c r="AMJ18" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="19" s="9">
-      <c r="A19" s="8" t="s">
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="19" s="10">
+      <c r="A19" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="G19" s="8"/>
-      <c r="H19" t="s">
+      <c r="G19" s="9"/>
+      <c r="H19" s="10" t="s">
         <v>23</v>
       </c>
       <c r="ALX19" s="0"/>
@@ -1320,25 +1326,25 @@
       <c r="AMI19" s="0"/>
       <c r="AMJ19" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="20" s="9">
-      <c r="A20" s="8" t="s">
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="20" s="10">
+      <c r="A20" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="E20" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E20" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" t="s">
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="10" t="s">
         <v>23</v>
       </c>
       <c r="ALX20" s="0"/>
@@ -1355,25 +1361,25 @@
       <c r="AMI20" s="0"/>
       <c r="AMJ20" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="21" s="9">
-      <c r="A21" s="8" t="s">
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="21" s="10">
+      <c r="A21" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="D21" s="8" t="s">
+      <c r="C21" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="G21" s="8"/>
-      <c r="H21" t="s">
+      <c r="E21" s="9"/>
+      <c r="F21" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G21" s="9"/>
+      <c r="H21" s="10" t="s">
         <v>23</v>
       </c>
       <c r="ALX21" s="0"/>
@@ -1390,7 +1396,7 @@
       <c r="AMI21" s="0"/>
       <c r="AMJ21" s="0"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="22" s="9">
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="22" s="10">
       <c r="A22" s="6" t="s">
         <v>7</v>
       </c>
@@ -1408,7 +1414,7 @@
         <v>27</v>
       </c>
       <c r="G22" s="6"/>
-      <c r="H22" t="s">
+      <c r="H22" s="10" t="s">
         <v>23</v>
       </c>
       <c r="ALX22" s="0"/>
@@ -1443,7 +1449,7 @@
         <v>31</v>
       </c>
       <c r="G23" s="6"/>
-      <c r="H23" t="s">
+      <c r="H23" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1458,16 +1464,16 @@
         <v>38</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="E24" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F24" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F24" s="6" t="s">
-        <v>41</v>
-      </c>
       <c r="G24" s="6"/>
-      <c r="H24" t="s">
+      <c r="H24" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1479,17 +1485,17 @@
         <v>32</v>
       </c>
       <c r="C25" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="E25" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
-      <c r="H25" t="s">
+      <c r="H25" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1501,153 +1507,153 @@
         <v>37</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>30</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G26" s="6"/>
-      <c r="H26" t="s">
+      <c r="H26" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="27">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8" t="s">
+      <c r="E27" s="9"/>
+      <c r="F27" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="G27" s="8"/>
-      <c r="H27" t="s">
+      <c r="G27" s="9"/>
+      <c r="H27" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="28">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8" t="s">
+      <c r="E28" s="9"/>
+      <c r="F28" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G28" s="8"/>
-      <c r="H28" t="s">
+      <c r="G28" s="9"/>
+      <c r="H28" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="29">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="D29" s="8" t="s">
+      <c r="C29" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E29" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F29" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="G29" s="8"/>
-      <c r="H29" t="s">
+      <c r="F29" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G29" s="9"/>
+      <c r="H29" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="30">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E30" s="8" t="s">
+      <c r="D30" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F30" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="G30" s="9"/>
+      <c r="H30" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="31">
+      <c r="A31" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="32">
+      <c r="A32" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="G30" s="8"/>
-      <c r="H30" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="31">
-      <c r="A31" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="32">
-      <c r="A32" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D32" s="8" t="s">
+      <c r="C32" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="G32" s="8"/>
-      <c r="H32" t="s">
+      <c r="E32" s="9"/>
+      <c r="F32" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G32" s="9"/>
+      <c r="H32" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1668,8 +1674,8 @@
       <c r="F33" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G33" s="10"/>
-      <c r="H33" t="s">
+      <c r="G33" s="11"/>
+      <c r="H33" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1690,8 +1696,8 @@
       <c r="F34" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G34" s="10"/>
-      <c r="H34" t="s">
+      <c r="G34" s="11"/>
+      <c r="H34" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1714,8 +1720,8 @@
       <c r="F35" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G35" s="10"/>
-      <c r="H35" t="s">
+      <c r="G35" s="11"/>
+      <c r="H35" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1727,19 +1733,19 @@
         <v>32</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G36" s="10"/>
-      <c r="H36" t="s">
+        <v>70</v>
+      </c>
+      <c r="G36" s="11"/>
+      <c r="H36" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1751,17 +1757,17 @@
         <v>37</v>
       </c>
       <c r="C37" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D37" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="E37" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E37" s="6" t="s">
-        <v>45</v>
-      </c>
       <c r="F37" s="6"/>
-      <c r="G37" s="10"/>
-      <c r="H37" t="s">
+      <c r="G37" s="11"/>
+      <c r="H37" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1770,271 +1776,271 @@
         <v>9</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>70</v>
+        <v>41</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>71</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>30</v>
       </c>
       <c r="E38" s="6"/>
       <c r="F38" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="G38" s="10"/>
-      <c r="H38" t="s">
+        <v>68</v>
+      </c>
+      <c r="G38" s="11"/>
+      <c r="H38" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="39">
-      <c r="A39" s="7" t="s">
+      <c r="A39" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C39" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D39" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7" t="s">
+      <c r="E39" s="8"/>
+      <c r="F39" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G39" s="7"/>
-      <c r="H39" t="s">
+      <c r="G39" s="8"/>
+      <c r="H39" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="40">
-      <c r="A40" s="7" t="s">
+      <c r="A40" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="C40" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7" t="s">
+      <c r="E40" s="8"/>
+      <c r="F40" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G40" s="7"/>
-      <c r="H40" t="s">
+      <c r="G40" s="8"/>
+      <c r="H40" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="41">
-      <c r="A41" s="7" t="s">
+      <c r="A41" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D41" s="7" t="s">
+      <c r="C41" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D41" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E41" s="7" t="s">
+      <c r="E41" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F41" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="G41" s="7"/>
-      <c r="H41" t="s">
+      <c r="F41" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G41" s="8"/>
+      <c r="H41" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="42">
-      <c r="A42" s="7" t="s">
+      <c r="A42" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B42" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C42" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G42" s="8"/>
+      <c r="H42" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="43">
+      <c r="A43" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="44">
+      <c r="A44" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D42" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="G42" s="7"/>
-      <c r="H42" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="43">
-      <c r="A43" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B43" s="7" t="s">
+      <c r="G44" s="8"/>
+      <c r="H44" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="45">
+      <c r="A45" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G45" s="9"/>
+      <c r="H45" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="46">
+      <c r="A46" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G46" s="9"/>
+      <c r="H46" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="47">
+      <c r="A47" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E47" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="48">
+      <c r="A48" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="49">
+      <c r="A49" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B49" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C43" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="44">
-      <c r="A44" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="G44" s="7"/>
-      <c r="H44" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="45">
-      <c r="A45" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E45" s="8"/>
-      <c r="F45" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="G45" s="8"/>
-      <c r="H45" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="46">
-      <c r="A46" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E46" s="8"/>
-      <c r="F46" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="G46" s="8"/>
-      <c r="H46" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="47">
-      <c r="A47" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E47" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="F47" s="8"/>
-      <c r="G47" s="8"/>
-      <c r="H47" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="48">
-      <c r="A48" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C48" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="D48" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E48" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="F48" s="8"/>
-      <c r="G48" s="8"/>
-      <c r="H48" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="49">
-      <c r="A49" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="D49" s="8" t="s">
+      <c r="C49" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="E49" s="8" t="s">
+      <c r="D49" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="F49" s="8"/>
-      <c r="G49" s="8"/>
-      <c r="H49" t="s">
+      <c r="E49" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="50">
-      <c r="A50" s="10" t="s">
+      <c r="A50" s="11" t="s">
         <v>12</v>
       </c>
       <c r="B50" s="6" t="s">
@@ -2050,13 +2056,13 @@
       <c r="F50" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G50" s="10"/>
+      <c r="G50" s="11"/>
       <c r="H50" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="51">
-      <c r="A51" s="10" t="s">
+      <c r="A51" s="11" t="s">
         <v>12</v>
       </c>
       <c r="B51" s="6" t="s">
@@ -2072,163 +2078,163 @@
       <c r="F51" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G51" s="10"/>
+      <c r="G51" s="11"/>
       <c r="H51" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="52">
-      <c r="A52" s="10" t="s">
+      <c r="A52" s="11" t="s">
         <v>12</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="F52" s="10"/>
-      <c r="G52" s="10"/>
+        <v>74</v>
+      </c>
+      <c r="F52" s="11"/>
+      <c r="G52" s="11"/>
       <c r="H52" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="53">
-      <c r="A53" s="10" t="s">
+      <c r="A53" s="11" t="s">
         <v>12</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>32</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="F53" s="10"/>
-      <c r="G53" s="10"/>
+        <v>77</v>
+      </c>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
       <c r="H53" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="54">
-      <c r="A54" s="10" t="s">
+      <c r="A54" s="11" t="s">
         <v>12</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>37</v>
       </c>
       <c r="C54" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F54" s="11"/>
+      <c r="G54" s="11"/>
+      <c r="H54" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="55">
+      <c r="A55" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E55" s="6" t="s">
         <v>77</v>
-      </c>
-      <c r="D54" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E54" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F54" s="10"/>
-      <c r="G54" s="10"/>
-      <c r="H54" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="55">
-      <c r="A55" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C55" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D55" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E55" s="6" t="s">
-        <v>76</v>
       </c>
       <c r="F55" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G55" s="10"/>
+      <c r="G55" s="11"/>
       <c r="H55" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="56">
-      <c r="A56" s="10" t="s">
+      <c r="A56" s="11" t="s">
         <v>12</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C56" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E56" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D56" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E56" s="6" t="s">
-        <v>79</v>
-      </c>
       <c r="F56" s="6"/>
-      <c r="G56" s="10"/>
+      <c r="G56" s="11"/>
       <c r="H56" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="57">
-      <c r="A57" s="10" t="s">
+      <c r="A57" s="11" t="s">
         <v>12</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C57" s="10" t="s">
-        <v>81</v>
+        <v>48</v>
+      </c>
+      <c r="C57" s="11" t="s">
+        <v>82</v>
       </c>
       <c r="D57" s="6" t="s">
         <v>30</v>
       </c>
       <c r="E57" s="6"/>
       <c r="F57" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="G57" s="10"/>
+        <v>83</v>
+      </c>
+      <c r="G57" s="11"/>
       <c r="H57" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="58">
-      <c r="A58" s="10" t="s">
+      <c r="A58" s="11" t="s">
         <v>12</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C58" s="10" t="s">
-        <v>83</v>
+        <v>52</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>84</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E58" s="6"/>
       <c r="F58" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="G58" s="10"/>
+        <v>83</v>
+      </c>
+      <c r="G58" s="11"/>
       <c r="H58" s="4" t="s">
         <v>23</v>
       </c>
@@ -2252,56 +2258,56 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A8" activeCellId="0" pane="topLeft" sqref="A8"/>
+      <selection activeCell="A8" activeCellId="1" pane="topLeft" sqref="C2:F8 A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="46.780612244898" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="0" width="27.4234693877551" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="0" width="27.1428571428571" collapsed="true"/>
-    <col min="4" max="4" hidden="false" style="0" width="18.5459183673469" collapsed="true"/>
-    <col min="5" max="5" hidden="false" style="0" width="11.8265306122449" collapsed="true"/>
-    <col min="6" max="1025" hidden="false" style="0" width="8.6734693877551" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.780612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.4234693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.1428571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.5459183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.8265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.6734693877551"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="B1" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="C1" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="D1" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>2</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="2">
-      <c r="A2" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="B2" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="C2" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="D2" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="mojio.2@optimusinfo.com" ref="B2" r:id="rId58"/>
+    <hyperlink display="mojio.2@optimusinfo.com" ref="B2" r:id="rId1"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2321,36 +2327,36 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B1" activeCellId="0" pane="topLeft" sqref="B1"/>
+      <selection activeCell="B1" activeCellId="1" pane="topLeft" sqref="C2:F8 B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="50.6734693877551" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="0" width="23.6530612244898" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="0" width="13.9744897959184" collapsed="true"/>
-    <col min="4" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.6734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.6530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.9744897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="C1" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="2">
-      <c r="A2" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="C2" s="11" t="s">
+      <c r="A2" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2373,41 +2379,41 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C1" activeCellId="0" pane="topLeft" sqref="C1"/>
+      <selection activeCell="C1" activeCellId="1" pane="topLeft" sqref="C2:F8 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="48.1224489795918" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="0" width="34.5408163265306" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="0" width="34.2704081632653" collapsed="true"/>
-    <col min="4" max="4" hidden="false" style="0" width="22.8520408163265" collapsed="true"/>
-    <col min="5" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.1224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.5408163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.2704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.8520408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="B1" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>93</v>
+      <c r="B1" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>94</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>2</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="2">
-      <c r="A2" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>94</v>
+      <c r="B2" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>95</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>4</v>
@@ -2415,7 +2421,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="mojio.2@optimusinfo.com" ref="B2" r:id="rId58"/>
+    <hyperlink display="mojio.2@optimusinfo.com" ref="B2" r:id="rId1"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2435,41 +2441,41 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C5" activeCellId="0" pane="topLeft" sqref="C5"/>
+      <selection activeCell="C5" activeCellId="0" pane="topLeft" sqref="C2:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="55.5102040816327" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="0" width="34.4030612244898" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="0" width="33.8724489795918" collapsed="true"/>
-    <col min="4" max="4" hidden="false" style="0" width="22.984693877551" collapsed="true"/>
-    <col min="5" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.5102040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.4030612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.8724489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.984693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>93</v>
+        <v>86</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>94</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>2</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="2">
-      <c r="A2" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>94</v>
+      <c r="A2" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>95</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>4</v>
@@ -2494,48 +2500,48 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D1" activeCellId="0" pane="topLeft" sqref="D1"/>
+      <selection activeCell="D1" activeCellId="1" pane="topLeft" sqref="C2:F8 D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="47.5816326530612" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="0" width="34.2704081632653" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="0" width="34.4030612244898" collapsed="true"/>
-    <col min="4" max="4" hidden="false" style="0" width="34.6734693877551" collapsed="true"/>
-    <col min="5" max="5" hidden="false" style="0" width="22.984693877551" collapsed="true"/>
-    <col min="6" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.5816326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.2704081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4030612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.6734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.984693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>87</v>
+        <v>96</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>88</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>2</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="2">
-      <c r="A2" s="11" t="s">
-        <v>89</v>
+      <c r="A2" s="12" t="s">
+        <v>90</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="D2" s="11" t="s">
         <v>98</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>99</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>4</v>
@@ -2560,48 +2566,48 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D1" activeCellId="0" pane="topLeft" sqref="D1"/>
+      <selection activeCell="D1" activeCellId="1" pane="topLeft" sqref="C2:F8 D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="48.1224489795918" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="0" width="34.5408163265306" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="0" width="34.0102040816326" collapsed="true"/>
-    <col min="4" max="4" hidden="false" style="0" width="34.2704081632653" collapsed="true"/>
-    <col min="5" max="5" hidden="false" style="0" width="23.2551020408163" collapsed="true"/>
-    <col min="6" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.1224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.5408163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.0102040816326"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.2704081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>99</v>
+        <v>87</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>100</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>2</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="2">
-      <c r="A2" s="11" t="s">
-        <v>89</v>
+      <c r="A2" s="12" t="s">
+        <v>90</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="C2" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>98</v>
+      <c r="C2" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>99</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>4</v>
@@ -2626,48 +2632,48 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D11" activeCellId="0" pane="topLeft" sqref="D11"/>
+      <selection activeCell="D11" activeCellId="1" pane="topLeft" sqref="C2:F8 D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="49.0663265306123" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="0" width="34.5408163265306" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="0" width="34.4030612244898" collapsed="true"/>
-    <col min="4" max="4" hidden="false" style="0" width="34.5408163265306" collapsed="true"/>
-    <col min="5" max="5" hidden="false" style="0" width="22.8520408163265" collapsed="true"/>
-    <col min="6" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.0663265306123"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.5408163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4030612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.5408163265306"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.8520408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>99</v>
+        <v>96</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>100</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>2</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="2">
-      <c r="A2" s="11" t="s">
-        <v>89</v>
+      <c r="A2" s="12" t="s">
+        <v>90</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="D2" s="11" t="s">
         <v>98</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>99</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>4</v>

</xml_diff>